<commit_message>
Edit scrape.R, pest.sci, agent.E
</commit_message>
<xml_diff>
--- a/agent_info_maiz.xlsx
+++ b/agent_info_maiz.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,15 +360,20 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>藥劑名稱</t>
+          <t>Agent.C</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Agent.E</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>每公頃使用量</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>稀釋倍數_x000D_
 							_x000D_
@@ -377,151 +382,188 @@
 							(倍)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>施藥方法</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>注意事項</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Pest</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Pest.Sci</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>24%納乃得溶液_x000D_
-							_x000D_
-							_x000D_
-							(Methomyl)</t>
+          <t xml:space="preserve">24%納乃得溶液_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Methomyl</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>0.9~1.2公升</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>生育初期，如發生蚜蟲平均每株100之時即行噴藥，每隔10天噴藥一次，計二至三次。</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>玉米-玉米蚜.htm</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>玉米蚜</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rhopalosiphum maidis </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>40.64%加保扶水懸劑_x000D_
-							_x000D_
-							_x000D_
-							(Carbofuran)</t>
+          <t xml:space="preserve">40.64%加保扶水懸劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Carbofuran</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>1.1~1.5公升</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>800</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>生育初期，如發生蚜蟲平均每株100之時即行噴藥，每隔10天噴藥一次，計二至三次。</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>玉米-玉米蚜.htm</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>玉米蚜</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rhopalosiphum maidis </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>諾伐隆100g/L乳劑_x000D_
-								_x000D_
-								_x000D_
-								(10%W/V)_x000D_
-								_x000D_
-								_x000D_
-								(Novaluron)</t>
+          <t xml:space="preserve">諾伐隆100g/L乳劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Novaluron</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>0.67公升</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>1,500</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>玉米輪生期、雄花抽穗期、吐絲初期各施藥一次。</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0.3%芬普尼粒劑_x000D_
-								_x000D_
-								_x000D_
-								(Fipronil)</t>
+          <t xml:space="preserve">0.3%芬普尼粒劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Fipronil</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>20公斤</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>1.生育初期發生玉米螟時，將藥粒施於心葉一次。_x000D_
 								_x000D_
 								_x000D_
@@ -531,7 +573,7 @@
 								3.每株用藥量0.4公克。</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>1.採收前15天停止施藥。_x000D_
 								_x000D_
@@ -542,323 +584,404 @@
 								3.對水生物具毒性，對蜜蜂毒性高。</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3.8%蘇力菌可濕性粉劑_x000D_
-								_x000D_
-								_x000D_
-								(Bacillus thuringiensis)</t>
+          <t xml:space="preserve">3.8%蘇力菌可濕性粉劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Bacillus thuringiensis</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>1公斤</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>於玉米輪生中期開始施藥，以後每隔7天施藥一次，共五次。</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>施藥時加展著劑「YAMATO」3,000倍於陰天或傍晚施藥。</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>蘇力菌(3200 IU/mg)水分散性粒劑_x000D_
-								_x000D_
-								_x000D_
-								(Bacillus thuringiensis)</t>
+          <t>蘇力菌</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Bacillus thuringiensis</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>0.3-0.4公斤</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>3,000</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>玉米苗高約30公分開始噴藥，隔7天再噴一次，另於雄花抽穗前7天去雄二分之一後、吐絲二分之一及全部吐絲，各再施藥一次。</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>施藥時加展著劑「力道威」2,000倍，於陰天或傍晚施藥。</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>蘇力菌(16000 IU/mg)粒劑_x000D_
-								_x000D_
-								_x000D_
-								(Bacillus thuringiensis)</t>
+          <t>蘇力菌</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Bacillus thuringiensis</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>5公斤</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>將藥粒平均施於心藥，分別於輪生初期；輪生中期；雄花抽穗前4-5天，雌花吐絲後3-4天，各施藥一次。</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>玉米-玉米螟.htm</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>蘇力菌(16000 IU/mg)可濕性粉劑_x000D_
-								_x000D_
-								_x000D_
-								(Bacillus thuringiensis)</t>
+          <t>蘇力菌</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Bacillus thuringiensis</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>1.6-2公斤</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>600</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>玉米輪生期、雄花抽穗期、吐絲初期、吐絲後期及全部吐絲後5天，各施藥一次。</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>施藥時加展著劑「YAMATO」3,000倍於陰天或傍晚施藥。</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20%依芬寧可濕性粉劑_x000D_
-								_x000D_
-								_x000D_
-								(Ethofenprox)</t>
+          <t xml:space="preserve">20%依芬寧可濕性粉劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Ethofenprox</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>0.67公斤</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>1,500</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>輪生期害蟲發生時施藥一次，雄花抽穗及幼穗期各再施藥一次。</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>採收前15天停止用藥。</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>50%加保利可濕性粉劑_x000D_
-								_x000D_
-								_x000D_
-								(Carbaryl)</t>
+          <t xml:space="preserve">50%加保利可濕性粉劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Carbaryl</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>2.4-2.8公斤</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>500</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>輪生期害蟲發生時抽穗後10天左右，如發生玉米螟時施藥一次，隔10天再施藥一次。</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>40.64%加保扶水懸劑_x000D_
-								_x000D_
-								_x000D_
-								(Carbofuran)</t>
+          <t xml:space="preserve">40.64%加保扶水懸劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Carbofuran</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>1.2-1.5公斤</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>800</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>輪生期害蟲發生時抽穗後10天左右，如發生玉米螟時施藥一次，隔10天再施藥一次。</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>玉米-玉米螟.htm</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3%加保扶粒劑_x000D_
-								_x000D_
-								_x000D_
-								(Carbofuran)</t>
+          <t xml:space="preserve">3%加保扶粒劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Carbofuran</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>40公斤</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>1.生育初期如發生玉米螟時，將藥粒施於心葉一次。_x000D_
 								_x000D_
 								_x000D_
 								2.雄花抽穗前10-15天，再將藥粒施於心葉一次。</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>採收前30天停止用藥。</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5%加保利粒劑_x000D_
-								_x000D_
-								_x000D_
-								(Carbaryl)</t>
+          <t xml:space="preserve">5%加保利粒劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Carbaryl</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>40公斤</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>1.生育初期如發生玉米螟時，將藥粒施於心葉一次。_x000D_
 								_x000D_
 								_x000D_
 								2.雄花抽穗前10-15天，再將藥粒施於心葉一次。</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>採收前15天停止用藥。_x000D_
 								_x000D_
@@ -866,40 +989,50 @@
 								*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5%陶斯松粒劑_x000D_
-								_x000D_
-								_x000D_
-								(Chlorpyrifos)</t>
+          <t xml:space="preserve">5%陶斯松粒劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Chlorpyrifos</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>20公斤</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>1.生育初期如發生玉米螟時，將藥粒施於心葉一次。_x000D_
 								_x000D_
 								_x000D_
 								2.雄花抽穗前10-15天，再將藥粒施於心葉一次。</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>1.每株用藥0.3-0.5公克。_x000D_
 								_x000D_
@@ -907,40 +1040,50 @@
 								2.採收前54天停止用藥。</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3%丁基加保扶粒劑_x000D_
-								_x000D_
-								_x000D_
-								(Carbosulfan)</t>
+          <t xml:space="preserve">3%丁基加保扶粒劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Carbosulfan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>40公斤</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>1.生育初期如發生玉米螟時，將藥粒施於心葉一次。_x000D_
 								_x000D_
 								_x000D_
 								2.雄花抽穗前10-15天，再將藥粒施於心葉一次。</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>1.每株施藥量0.87公克。_x000D_
 								_x000D_
@@ -955,129 +1098,164 @@
 								*丁基加保扶為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>85%加保利可濕性粉劑_x000D_
-								_x000D_
-								_x000D_
-								(Carbaryl)</t>
+          <t xml:space="preserve">85%加保利可濕性粉劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>Carbaryl</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>1.4-1.6公斤</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>850</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>玉米-玉米螟.htm</t>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>玉米螟</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ostrinia furnacalis </t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5％護賽寧乳劑_x000D_
-								_x000D_
-								_x000D_
-								(Flucythrinate)</t>
+          <t xml:space="preserve">5％護賽寧乳劑_x000D_
+								_x000D_
+								_x000D_
+								</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Flucythrinate</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>1公斤</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>800</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>藥劑應噴灑於玉米葉片上、下兩面。</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>採收前15天停止施藥。</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>玉米-玉米薊馬.htm</t>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>玉米薊馬</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Frankliniella williamsi</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5％護賽寧乳劑_x000D_
+          <t xml:space="preserve">5％護賽寧乳劑_x000D_
 										_x000D_
 										_x000D_
-										(Flucythrinate)</t>
+										</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Flucythrinate</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>800</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>蟲害發生時開始施藥，每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>採收前15天停止施藥。</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>玉米-甜菜夜蛾.htm</t>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>甜菜夜蛾</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Spodoptera exigua</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>80.2%甜菜夜蛾費洛蒙蒸散劑_x000D_
-									_x000D_
-									_x000D_
-									(sex pheromones of Spodoptera exigua)</t>
+          <t xml:space="preserve">80.2%甜菜夜蛾費洛蒙蒸散劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>sex pheromones of Spodoptera exigua</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1087,6 +1265,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>1.每公頃設置點數11至18個，每個點前後距離約30公尺，左右距離約15公尺。_x000D_
 									_x000D_
 									_x000D_
@@ -1099,7 +1282,7 @@
 									4.誘蟲盒以中改式誘蟲盒；制式誘蟲盒或利用廢棄寶特瓶自行加開誘蟲口。</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>1.本性費洛蒙引誘劑是以塑膠微管為載體，每支誘餌內裝劑量為5毫克。_x000D_
 									_x000D_
@@ -1116,32 +1299,42 @@
 									5.溫度低於攝氏15℃以下或雨季連續下雨時，因蟲口數降低，暫緩施設。</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>玉米-甜菜夜蛾.htm</t>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>甜菜夜蛾</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Spodoptera exigua</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5%護賽寧溶液_x000D_
+          <t xml:space="preserve">5%護賽寧溶液_x000D_
 										_x000D_
 										_x000D_
-										(Flucythrinate)</t>
+										</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>Flucythrinate</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>1.0公升</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>800</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>1.生育初期，如發生穗夜蛾即行施藥，每隔10天施藥一次計二至三次。_x000D_
 										_x000D_
@@ -1149,37 +1342,47 @@
 										2.在抽穗後，開花初期，於穗部施藥一次，經10天後如再發生，再施藥一次(務必噴及穗部)。</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>採收前15天停止施藥。</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>玉米-番茄夜蛾.htm</t>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>番茄夜蛾</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Helicoverpa armigera</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>40.64%加保扶水懸劑_x000D_
+          <t xml:space="preserve">40.64%加保扶水懸劑_x000D_
 										_x000D_
 										_x000D_
-										(Carbofuran)</t>
+										</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Carbofuran</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>1.1-1.5公升</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>800</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>1.生育初期，如發生穗夜蛾即行施藥，每隔10天施藥一次計二至三次。_x000D_
 										_x000D_
@@ -1187,37 +1390,47 @@
 										2.在抽穗後，開花初期，於穗部施藥一次，經10天後如再發生，再施藥一次(務必噴及穗部)。</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>使用前將藥瓶上下搖動，使藥液均勻。</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>玉米-番茄夜蛾.htm</t>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>番茄夜蛾</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Helicoverpa armigera</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>50%加保利可濕性粉劑_x000D_
+          <t xml:space="preserve">50%加保利可濕性粉劑_x000D_
 										_x000D_
 										_x000D_
-										(Carbaryl)</t>
+										</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>Carbaryl</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>1.6公斤</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>500</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>1.生育初期，如發生穗夜蛾即行施藥，每隔10天施藥一次計二至三次。_x000D_
 										_x000D_
@@ -1225,147 +1438,187 @@
 										2.在抽穗後，開花初期，於穗部施藥一次，經10天後如再發生，再施藥一次(務必噴及穗部)。</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>玉米-番茄夜蛾.htm</t>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>番茄夜蛾</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Helicoverpa armigera</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>85%加保利可濕性粉劑_x000D_
+          <t xml:space="preserve">85%加保利可濕性粉劑_x000D_
 										_x000D_
 										_x000D_
-										(Carbofuran)</t>
+										</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>Carbofuran</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>1.1-1.5公斤</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>850</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>玉米-番茄夜蛾.htm</t>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>番茄夜蛾</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Helicoverpa armigera</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2.8%第滅寧水基乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Deltamethrin)</t>
+          <t xml:space="preserve">2.8%第滅寧水基乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>Deltamethrin</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>0.7公升</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>2,000</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>於蝗蝻發生初期施藥，每隔7天施藥一次，連續一至二次。</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>採收前6天停止施藥。</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>玉米-玉米條背土蝗.htm</t>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>玉米條背土蝗</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patanga succincta </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2.8%第滅寧乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Deltamethrin)</t>
+          <t xml:space="preserve">2.8%第滅寧乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>Deltamethrin</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>0.7公升</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>2,000</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>於蝗蝻發生初期施藥，每隔7天施藥一次，連續一至二次。</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>採收前6天停止施藥。</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>玉米-玉米條背土蝗.htm</t>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>玉米條背土蝗</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patanga succincta </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>50%撲滅松乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Fenitrothion)</t>
+          <t xml:space="preserve">50%撲滅松乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>Fenitrothion</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>1.0公升</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>於蝗蝻發生初期施藥，每隔7天施藥一次，連續一至二次。</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>1.採收前6天停止施藥。_x000D_
 							_x000D_
@@ -1373,282 +1626,362 @@
 							2.對蜜蜂輕毒，對水生物具毒性，勿使用於「飲用水水源水質保護區」及「飲用水取水口一定距離內之地區」。</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>玉米-玉米條背土蝗.htm</t>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>玉米條背土蝗</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patanga succincta </t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>85%加保利可濕性粉劑_x000D_
-							_x000D_
-							_x000D_
-							(Carbaryl)</t>
+          <t xml:space="preserve">85%加保利可濕性粉劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>Carbaryl</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>1.5公斤</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E28" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
           <t>*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>玉米-玉米條背土蝗.htm</t>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>玉米條背土蝗</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patanga succincta </t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2%依殺松粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Isazofos)</t>
+          <t xml:space="preserve">2%依殺松粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>Isazofos</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>40公斤</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>種植後地面施藥一次，以後每隔10天施藥一次，連續施藥二次。</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>對水生物劇毒性，並禁用於水域、空中施藥及大面積施用(高爾夫球場在內)。</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3%加福松微粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Isoxathion)</t>
+          <t xml:space="preserve">3%加福松微粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>Isoxathion</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>50公斤</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D30" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>限定植前施藥。</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5%免扶克粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Benfuracarb)</t>
+          <t xml:space="preserve">5%免扶克粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>Benfuracarb</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>30公斤</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>採收前28天停止施藥。</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>22.5%陶斯松乳劑_x000D_
-									_x000D_
-									_x000D_
-									(Chlorpyrifos)</t>
+          <t xml:space="preserve">22.5%陶斯松乳劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>Chlorpyrifos</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>1.5公升</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>700</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>種植後地面施藥一次，以後每隔10天施藥一次，連續施藥二次。</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>40.8%陶斯松乳劑_x000D_
-									_x000D_
-									_x000D_
-									(Chlorpyrifos)</t>
+          <t xml:space="preserve">40.8%陶斯松乳劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>Chlorpyrifos</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>1.2公升</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>種植後地面施藥一次，以後每隔10天施藥一次，連續施藥二次。</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>40.64%加保扶水懸劑_x000D_
-									_x000D_
-									_x000D_
-									(Carbofuran)</t>
+          <t xml:space="preserve">40.64%加保扶水懸劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Carbofuran</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>1,200</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E34" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
           <t>採收前15天停止施藥。</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3%加保扶粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Carbofuran)</t>
+          <t xml:space="preserve">3%加保扶粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>Carbofuran</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>50公斤</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>1.施藥時必須戴手套。_x000D_
 									_x000D_
@@ -1656,37 +1989,47 @@
 									2.種植前施藥一次，生育期不可施藥。</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3%安殺番粉劑_x000D_
-									_x000D_
-									_x000D_
-									(Endosulfan)</t>
+          <t xml:space="preserve">3%安殺番粉劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>Endosulfan</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>40-50公斤</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D36" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>1.採收前14天停止施藥。 _x000D_
 									_x000D_
@@ -1698,72 +2041,92 @@
 									3.不可與皮膚接觸。</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0.5%芬化利粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Fenvalerate)</t>
+          <t xml:space="preserve">0.5%芬化利粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>Fenvalerate</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>50公斤</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D37" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>種植前3天及定植後3天、10天各在畦上施藥一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>施藥時必須戴手套。</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2%加福松粉劑_x000D_
-									_x000D_
-									_x000D_
-									(Isoxathion)</t>
+          <t xml:space="preserve">2%加福松粉劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>Isoxathion</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>40公斤</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D38" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
           <t>種植前3天及定植後3天、10天各在畦上施藥一次，隔一星期再施藥一次，並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>1.施藥時必須戴手套。_x000D_
 									_x000D_
@@ -1771,142 +2134,182 @@
 									2.採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5%陶斯松粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Chlorpyrifos)</t>
+          <t xml:space="preserve">5%陶斯松粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>Chlorpyrifos</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>30公斤</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D39" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分，定植後一週再施藥一次。</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>10%托福松粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Terbufos)</t>
+          <t xml:space="preserve">10%托福松粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>Terbufos</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>10公斤</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>限播種時使用。</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>45%普伏松乳劑_x000D_
-									_x000D_
-									_x000D_
-									(Ethoprop)</t>
+          <t xml:space="preserve">45%普伏松乳劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>Ethoprop</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>3公升</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>300</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>限包葉菜類生長初期使用。</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3%丁基加保扶粒劑_x000D_
-									_x000D_
-									_x000D_
-									(Carbosulfan)</t>
+          <t xml:space="preserve">3%丁基加保扶粒劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>Carbosulfan</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>40公斤</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="D42" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>種植前3天在畦上撒佈一次並以鐵耙拌土約5公分。</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>1.限播種前使用。_x000D_
 									_x000D_
@@ -1917,648 +2320,830 @@
 									3.採收時剝去之外葉不得使用，應予燬棄。</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>玉米-切根蟲.htm</t>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>25%陶斯寧乳劑_x000D_
-									_x000D_
-									_x000D_
-									(Chlorpyrifos+_x000D_
-									_x000D_
-									_x000D_
-									Cypermethrin)</t>
+          <t xml:space="preserve">25%陶斯寧乳劑_x000D_
+									_x000D_
+									_x000D_
+									</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>Chlorpyrifos+_x000D_
+									_x000D_
+									_x000D_
+									Cypermethrin</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>0.7-1公升</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>定植前3天施藥一次。</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>玉米-切根蟲.htm</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>切根蟲</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Agrotis ipsilon</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>58%乃力松乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Naled)</t>
+          <t xml:space="preserve">58%乃力松乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>Naled</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>0.5-1公升</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>每隔7至10天施藥一次。</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>採收前4天停止施藥。</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>25%拜裕松乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Quinalphos)</t>
+          <t xml:space="preserve">25%拜裕松乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>Quinalphos</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>1-2公升</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>500</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>每隔7至10天施藥一次。</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>26.3%亞特松乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Pirimiphosmethyl)</t>
+          <t xml:space="preserve">26.3%亞特松乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>Pirimiphosmethyl</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>0.15-0.25公升</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>500</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>每隔7至10天施藥一次。</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20%芬化利水基乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Fenvalerate)</t>
+          <t xml:space="preserve">20%芬化利水基乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>Fenvalerate</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>0.15-0.25公升</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>3,000</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>採收前14天停止施藥。</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20%芬化利乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Fenvalerate)</t>
+          <t xml:space="preserve">20%芬化利乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>Fenvalerate</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>0.15-0.25公升</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>3,000</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>採收前14天停止施藥。</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20%芬化利可濕性粉劑_x000D_
-							_x000D_
-							_x000D_
-							(Fenvalerate)</t>
+          <t xml:space="preserve">20%芬化利可濕性粉劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Fenvalerate</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
           <t>5,000</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>每隔7至10天施藥一次。</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20%芬化利片劑_x000D_
-							_x000D_
-							_x000D_
-							(Fenvalerate)</t>
+          <t xml:space="preserve">20%芬化利片劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Fenvalerate</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
           <t>5,000</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>每隔7至10天施藥一次。</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>採收前7天停止施藥。</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5%芬化利乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Fenvalerate)</t>
+          <t xml:space="preserve">5%芬化利乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>Fenvalerate</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>0.5公升</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>2,000</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>採收前10天停止施藥。</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3%蘇力菌可濕性粉劑(每公克含300億孢子)_x000D_
-							_x000D_
-							_x000D_
-							(Bacillus thuringiensis)</t>
+          <t>3%蘇力菌可濕性粉劑</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>Bacillus thuringiensis</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>0.4-0.6公斤</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>1,500</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>採收前亦可施用。</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>40.64%加保扶水懸劑_x000D_
-							_x000D_
-							_x000D_
-							(Carbofuran)</t>
+          <t xml:space="preserve">40.64%加保扶水懸劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Carbofuran</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>1,200</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>採收前15天停止施藥。</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>10%百滅寧可濕性粉劑_x000D_
-							_x000D_
-							_x000D_
-							(Permethrin)</t>
+          <t xml:space="preserve">10%百滅寧可濕性粉劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Permethrin</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
           <t>3,000</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>採收前2-4天停止施藥。</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>10%百滅寧乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Permethrin)</t>
+          <t xml:space="preserve">10%百滅寧乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Permethrin</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
           <t>3,000</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="F55" t="inlineStr">
         <is>
           <t>採收前2-4天停止施藥。</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5%賽滅寧可濕性粉劑_x000D_
-							_x000D_
-							_x000D_
-							(Cypermethrin)</t>
+          <t xml:space="preserve">5%賽滅寧可濕性粉劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Cypermethrin</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
           <t>1,500</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="F56" t="inlineStr">
         <is>
           <t>採收前6天停止施藥。</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5%賽滅寧微乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Cypermethrin)</t>
+          <t xml:space="preserve">5%賽滅寧微乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Cypermethrin</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
           <t>1,500</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>每隔7天施藥一次。</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>採收前6天停止施藥。</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5%賽滅寧乳劑_x000D_
-							_x000D_
-							_x000D_
-							(Cypermethrin)</t>
+          <t xml:space="preserve">5%賽滅寧乳劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Cypermethrin</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
           <t>1,500</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E58" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
           <t>採收前6天停止施藥。</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>50%加保利可濕性粉劑_x000D_
-							_x000D_
-							_x000D_
-							(Carbaryl)</t>
+          <t xml:space="preserve">50%加保利可濕性粉劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Carbaryl</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
           <t>1,000</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E59" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
           <t>採收前7天停止施藥。_x000D_
 							_x000D_
 							_x000D_
 							*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>85%加保利可濕性粉劑_x000D_
-							_x000D_
-							_x000D_
-							(Carbaryl)</t>
+          <t xml:space="preserve">85%加保利可濕性粉劑_x000D_
+							_x000D_
+							_x000D_
+							</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Carbaryl</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
           <t>1,700</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E60" t="inlineStr">
         <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
           <t>採收前7天停止施藥。_x000D_
 							_x000D_
 							_x000D_
 							*加保利為限制登記使用農藥，不接受擴大作物範圍申請。</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>玉米-擬尺蠖.htm</t>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>擬尺蠖</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trichoplusia ni </t>
         </is>
       </c>
     </row>

</xml_diff>